<commit_message>
Liste des users stories
</commit_message>
<xml_diff>
--- a/divers/web_base-backlog_items_154.xlsx
+++ b/divers/web_base-backlog_items_154.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10309"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/vinoPerso/divers/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CMaisonneuve\582-N61\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB377D2-9F4F-424F-83B2-30509BF40F05}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="30060" windowHeight="14900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -140,7 +139,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="##0"/>
   </numFmts>
@@ -161,18 +160,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -187,7 +180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -195,9 +188,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -293,23 +283,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -345,23 +318,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -537,21 +493,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.33203125" customWidth="1"/>
-    <col min="3" max="3" width="60.5" style="4" customWidth="1"/>
-    <col min="4" max="4" width="94.1640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="60.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="94.140625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -565,7 +521,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>317929</v>
       </c>
@@ -579,7 +535,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>318830</v>
       </c>
@@ -593,7 +549,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>317927</v>
       </c>
@@ -607,7 +563,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>317926</v>
       </c>
@@ -621,7 +577,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>318829</v>
       </c>
@@ -635,49 +591,49 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>317930</v>
       </c>
       <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>317931</v>
       </c>
       <c r="B8" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>317933</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>317934</v>
       </c>
@@ -691,7 +647,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>317935</v>
       </c>
@@ -705,63 +661,63 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>317936</v>
       </c>
       <c r="B12" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>317937</v>
       </c>
       <c r="B13" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>23</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>317938</v>
       </c>
       <c r="B14" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>317939</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="4" t="s">
         <v>25</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="160" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="150" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>317940</v>
       </c>
@@ -775,7 +731,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>317941</v>
       </c>
@@ -789,7 +745,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>317942</v>
       </c>
@@ -803,28 +759,28 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>317943</v>
       </c>
       <c r="B19" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>317945</v>
       </c>
       <c r="B20" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D20" s="4" t="s">
@@ -832,7 +788,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D20">
+  <sortState ref="A2:D20">
     <sortCondition ref="B2:B20"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>